<commit_message>
revisi P3P Agustus 2020
</commit_message>
<xml_diff>
--- a/2020AgtP3P_S3P.xlsx
+++ b/2020AgtP3P_S3P.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
   <si>
     <t>P3P/S3P = Pagi 3 Pasal / Sore 3 Pasal</t>
   </si>
@@ -235,6 +235,24 @@
   </si>
   <si>
     <t>Yeh 4</t>
+  </si>
+  <si>
+    <t>Ams 11</t>
+  </si>
+  <si>
+    <t>Mzm 74</t>
+  </si>
+  <si>
+    <t>Luk 2</t>
+  </si>
+  <si>
+    <t>Hak 12</t>
+  </si>
+  <si>
+    <t>1 Kor 9</t>
+  </si>
+  <si>
+    <t>Yeh 5</t>
   </si>
 </sst>
 </file>
@@ -575,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +673,18 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -663,6 +693,12 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
+      <c r="H5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -670,6 +706,12 @@
       </c>
       <c r="D6" t="s">
         <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
revisi lagi P3P Agustus 2020
</commit_message>
<xml_diff>
--- a/2020AgtP3P_S3P.xlsx
+++ b/2020AgtP3P_S3P.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="134">
   <si>
     <t>P3P/S3P = Pagi 3 Pasal / Sore 3 Pasal</t>
   </si>
@@ -253,6 +253,171 @@
   </si>
   <si>
     <t>Yeh 5</t>
+  </si>
+  <si>
+    <t>Ams 12</t>
+  </si>
+  <si>
+    <t>Mzm 75</t>
+  </si>
+  <si>
+    <t>Luk 3</t>
+  </si>
+  <si>
+    <t>Hak 13</t>
+  </si>
+  <si>
+    <t>1 Kor 10</t>
+  </si>
+  <si>
+    <t>Yeh 6</t>
+  </si>
+  <si>
+    <t>Ams 13</t>
+  </si>
+  <si>
+    <t>Mzm 76</t>
+  </si>
+  <si>
+    <t>Luk 4</t>
+  </si>
+  <si>
+    <t>Hak 14</t>
+  </si>
+  <si>
+    <t>1 Kor 11</t>
+  </si>
+  <si>
+    <t>Yeh 7</t>
+  </si>
+  <si>
+    <t>Ams 14</t>
+  </si>
+  <si>
+    <t>Mzm 77</t>
+  </si>
+  <si>
+    <t>Luk 5</t>
+  </si>
+  <si>
+    <t>Hak 15</t>
+  </si>
+  <si>
+    <t>1 Kor 12</t>
+  </si>
+  <si>
+    <t>Yeh 8</t>
+  </si>
+  <si>
+    <t>Ams 15</t>
+  </si>
+  <si>
+    <t>Mzm 78</t>
+  </si>
+  <si>
+    <t>Luk 6</t>
+  </si>
+  <si>
+    <t>Hak 16</t>
+  </si>
+  <si>
+    <t>1 Kor 13</t>
+  </si>
+  <si>
+    <t>Yeh 9</t>
+  </si>
+  <si>
+    <t>Ams 16</t>
+  </si>
+  <si>
+    <t>Mzm 79</t>
+  </si>
+  <si>
+    <t>Luk 7</t>
+  </si>
+  <si>
+    <t>Hak 17</t>
+  </si>
+  <si>
+    <t>1 Kor 14</t>
+  </si>
+  <si>
+    <t>Yeh 10</t>
+  </si>
+  <si>
+    <t>Ams 17</t>
+  </si>
+  <si>
+    <t>Mzm 80</t>
+  </si>
+  <si>
+    <t>Luk 8</t>
+  </si>
+  <si>
+    <t>Hak 18</t>
+  </si>
+  <si>
+    <t>1 Kor 15</t>
+  </si>
+  <si>
+    <t>Yeh 11</t>
+  </si>
+  <si>
+    <t>Ams 18</t>
+  </si>
+  <si>
+    <t>Mzm 81</t>
+  </si>
+  <si>
+    <t>Luk 9</t>
+  </si>
+  <si>
+    <t>Hak 19</t>
+  </si>
+  <si>
+    <t>1 Kor 16</t>
+  </si>
+  <si>
+    <t>Yeh 12</t>
+  </si>
+  <si>
+    <t>Ams 19</t>
+  </si>
+  <si>
+    <t>Mzm 82</t>
+  </si>
+  <si>
+    <t>Luk 10</t>
+  </si>
+  <si>
+    <t>Hak 20</t>
+  </si>
+  <si>
+    <t>Yeh 13</t>
+  </si>
+  <si>
+    <t>2 Kor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamis </t>
+  </si>
+  <si>
+    <t>Ams 20</t>
+  </si>
+  <si>
+    <t>Mzm 83</t>
+  </si>
+  <si>
+    <t>Luk 11</t>
+  </si>
+  <si>
+    <t>Hak 21</t>
+  </si>
+  <si>
+    <t>2 Kor 2</t>
+  </si>
+  <si>
+    <t>Yeh 14</t>
   </si>
 </sst>
 </file>
@@ -594,7 +759,7 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,6 +892,18 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
@@ -735,6 +912,12 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
+      <c r="H9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
@@ -743,6 +926,12 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
+      <c r="H10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -757,6 +946,18 @@
       <c r="D12" t="s">
         <v>22</v>
       </c>
+      <c r="F12">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
@@ -765,6 +966,12 @@
       <c r="D13" t="s">
         <v>24</v>
       </c>
+      <c r="H13" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
@@ -773,6 +980,12 @@
       <c r="D14" t="s">
         <v>26</v>
       </c>
+      <c r="H14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -787,24 +1000,48 @@
       <c r="D16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>30</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>32</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -817,24 +1054,48 @@
       <c r="D20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>37</v>
       </c>
       <c r="D21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>39</v>
       </c>
       <c r="D22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -847,24 +1108,48 @@
       <c r="D24" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>44</v>
       </c>
       <c r="D25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>46</v>
       </c>
       <c r="D26" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -877,24 +1162,48 @@
       <c r="D28" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>17</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>51</v>
       </c>
       <c r="D29" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>111</v>
+      </c>
+      <c r="I29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>53</v>
       </c>
       <c r="D30" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>8</v>
       </c>
@@ -907,24 +1216,48 @@
       <c r="D32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" t="s">
+        <v>115</v>
+      </c>
+      <c r="I32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>57</v>
       </c>
       <c r="D33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>117</v>
+      </c>
+      <c r="I33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>59</v>
       </c>
       <c r="D34" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9</v>
       </c>
@@ -937,24 +1270,48 @@
       <c r="D36" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>19</v>
+      </c>
+      <c r="G36" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" t="s">
+        <v>121</v>
+      </c>
+      <c r="I36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>63</v>
       </c>
       <c r="D37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>123</v>
+      </c>
+      <c r="I37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>65</v>
       </c>
       <c r="D38" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>126</v>
+      </c>
+      <c r="I38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10</v>
       </c>
@@ -967,21 +1324,45 @@
       <c r="D40" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>20</v>
+      </c>
+      <c r="G40" t="s">
+        <v>127</v>
+      </c>
+      <c r="H40" t="s">
+        <v>128</v>
+      </c>
+      <c r="I40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>69</v>
       </c>
       <c r="D41" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>130</v>
+      </c>
+      <c r="I41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>71</v>
       </c>
       <c r="D42" t="s">
         <v>72</v>
+      </c>
+      <c r="H42" t="s">
+        <v>132</v>
+      </c>
+      <c r="I42" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Box Border P3P Agustus 2020
</commit_message>
<xml_diff>
--- a/2020AgtP3P_S3P.xlsx
+++ b/2020AgtP3P_S3P.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="200">
   <si>
     <t>P3P/S3P = Pagi 3 Pasal / Sore 3 Pasal</t>
   </si>
@@ -418,14 +418,220 @@
   </si>
   <si>
     <t>Yeh 14</t>
+  </si>
+  <si>
+    <t>Ams 21</t>
+  </si>
+  <si>
+    <t>Luk 12</t>
+  </si>
+  <si>
+    <t>2 Kor 3</t>
+  </si>
+  <si>
+    <t>Mzm 84</t>
+  </si>
+  <si>
+    <t>Rut 1</t>
+  </si>
+  <si>
+    <t>Yeh 15</t>
+  </si>
+  <si>
+    <t>Ams 22</t>
+  </si>
+  <si>
+    <t>Luk 13</t>
+  </si>
+  <si>
+    <t>2 Kor 4</t>
+  </si>
+  <si>
+    <t>Mzm 85</t>
+  </si>
+  <si>
+    <t>Rut 2</t>
+  </si>
+  <si>
+    <t>Yeh 16</t>
+  </si>
+  <si>
+    <t>Ams 23</t>
+  </si>
+  <si>
+    <t>Luk 14</t>
+  </si>
+  <si>
+    <t>2 Kor 5</t>
+  </si>
+  <si>
+    <t>Mzm 86</t>
+  </si>
+  <si>
+    <t>Yeh 17</t>
+  </si>
+  <si>
+    <t>Ams 24</t>
+  </si>
+  <si>
+    <t>Luk 15</t>
+  </si>
+  <si>
+    <t>2 Kor 6</t>
+  </si>
+  <si>
+    <t>Mzm 87</t>
+  </si>
+  <si>
+    <t>Rut 3</t>
+  </si>
+  <si>
+    <t>Yeh 18</t>
+  </si>
+  <si>
+    <t>Ams 25</t>
+  </si>
+  <si>
+    <t>Luk 16</t>
+  </si>
+  <si>
+    <t>Mzm 88</t>
+  </si>
+  <si>
+    <t>Rut 4</t>
+  </si>
+  <si>
+    <t>Yeh 19</t>
+  </si>
+  <si>
+    <t>Ams 26</t>
+  </si>
+  <si>
+    <t>Luk 17</t>
+  </si>
+  <si>
+    <t>Mzm 89</t>
+  </si>
+  <si>
+    <t>1 Sam 1</t>
+  </si>
+  <si>
+    <t>Yeh 20</t>
+  </si>
+  <si>
+    <t>Ams 27</t>
+  </si>
+  <si>
+    <t>Luk 18</t>
+  </si>
+  <si>
+    <t>Mzm 90</t>
+  </si>
+  <si>
+    <t>1 Sam 2</t>
+  </si>
+  <si>
+    <t>Yeh 21</t>
+  </si>
+  <si>
+    <t>Ams 28</t>
+  </si>
+  <si>
+    <t>Luk 19</t>
+  </si>
+  <si>
+    <t>2 Kor 7</t>
+  </si>
+  <si>
+    <t>Mzm 91</t>
+  </si>
+  <si>
+    <t>1 Sam 3</t>
+  </si>
+  <si>
+    <t>Yeh 22</t>
+  </si>
+  <si>
+    <t>Ams 29</t>
+  </si>
+  <si>
+    <t>Luk 20</t>
+  </si>
+  <si>
+    <t>2 Kor 8</t>
+  </si>
+  <si>
+    <t>Mzm 92</t>
+  </si>
+  <si>
+    <t>1 Sam 4</t>
+  </si>
+  <si>
+    <t>Yeh 23</t>
+  </si>
+  <si>
+    <t>Ams 30</t>
+  </si>
+  <si>
+    <t>Luk 21</t>
+  </si>
+  <si>
+    <t>2 Kor 9</t>
+  </si>
+  <si>
+    <t>Mzm 93</t>
+  </si>
+  <si>
+    <t>1 Sam 5</t>
+  </si>
+  <si>
+    <t>Yeh 24</t>
+  </si>
+  <si>
+    <t>Ams 31</t>
+  </si>
+  <si>
+    <t>Luk 22</t>
+  </si>
+  <si>
+    <t>Mzm 94</t>
+  </si>
+  <si>
+    <t>1 Sam 6</t>
+  </si>
+  <si>
+    <t>Yeh 25</t>
+  </si>
+  <si>
+    <t>2 Kor 10</t>
+  </si>
+  <si>
+    <t>2 Kor 11</t>
+  </si>
+  <si>
+    <t>2 Kor 12</t>
+  </si>
+  <si>
+    <t>2 Kor 13</t>
+  </si>
+  <si>
+    <t>1 Sam 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -441,7 +647,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -449,12 +655,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,617 +1056,1330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="B1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="2.28515625" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="2.28515625" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" customWidth="1"/>
+    <col min="14" max="15" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5"/>
+      <c r="G4" s="4">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="4">
+        <v>21</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="K6" s="5"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5"/>
+      <c r="G8" s="2">
         <v>12</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="2">
+        <v>22</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H9" t="s">
+      <c r="F9" s="5"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="K9" s="5"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H10" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="K10" s="5"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5"/>
+      <c r="G12" s="2">
         <v>13</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="2">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="M12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H13" t="s">
+      <c r="F13" s="5"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="K13" s="5"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H14" t="s">
+      <c r="F14" s="5"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="K14" s="5"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="5"/>
+      <c r="G16" s="2">
         <v>14</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="K16" s="5"/>
+      <c r="L16" s="2">
+        <v>24</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H17" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="K17" s="5"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H18" t="s">
+      <c r="F18" s="5"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="K18" s="5"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
         <v>5</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="5"/>
+      <c r="G20" s="2">
         <v>15</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="K20" s="5"/>
+      <c r="L20" s="2">
+        <v>25</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H21" t="s">
+      <c r="F21" s="5"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="K21" s="5"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H22" t="s">
+      <c r="F22" s="5"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="K22" s="5"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
         <v>6</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="5"/>
+      <c r="G24" s="2">
         <v>16</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="K24" s="5"/>
+      <c r="L24" s="2">
+        <v>26</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H25" t="s">
+      <c r="F25" s="5"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="K25" s="5"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H26" t="s">
+      <c r="F26" s="5"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="K26" s="5"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
         <v>7</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="5"/>
+      <c r="G28" s="2">
         <v>17</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="K28" s="5"/>
+      <c r="L28" s="2">
+        <v>27</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H29" t="s">
+      <c r="F29" s="5"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="K29" s="5"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H30" t="s">
+      <c r="F30" s="5"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="K30" s="5"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
         <v>8</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="5"/>
+      <c r="G32" s="2">
         <v>18</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="K32" s="5"/>
+      <c r="L32" s="2">
+        <v>28</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H33" t="s">
+      <c r="F33" s="5"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="K33" s="5"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H34" t="s">
+      <c r="F34" s="5"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="K34" s="5"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
         <v>9</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="5"/>
+      <c r="G36" s="2">
         <v>19</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+      <c r="K36" s="5"/>
+      <c r="L36" s="2">
+        <v>29</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H37" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="K37" s="5"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H38" t="s">
+      <c r="F38" s="5"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="K38" s="5"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
         <v>10</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="5"/>
+      <c r="G40" s="2">
         <v>20</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="K40" s="5"/>
+      <c r="L40" s="2">
+        <v>30</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H41" t="s">
+      <c r="F41" s="5"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+      <c r="K41" s="5"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H42" t="s">
+      <c r="F42" s="5"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="K42" s="5"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K44" s="11"/>
+      <c r="L44" s="2">
+        <v>31</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>194</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="92">
+    <mergeCell ref="L44:L46"/>
+    <mergeCell ref="M44:M46"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="L43:O43"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="M40:M42"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="L36:L38"/>
+    <mergeCell ref="M36:M38"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="M28:M30"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="M24:M26"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="M16:M18"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="K3:K43"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="F3:F43"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B27:E27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>